<commit_message>
Ajuste planilha de requisito
</commit_message>
<xml_diff>
--- a/Trabalho MVP - Grupo 8.xlsx
+++ b/Trabalho MVP - Grupo 8.xlsx
@@ -213,64 +213,68 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -579,219 +583,219 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.63671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="87.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="87.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C18"/>

</xml_diff>